<commit_message>
checkpoint, can run now. Add database cleanup script for corrupted golden_citations data; update Java version to 21; enhance Excel parsing service with unchecked exception handling; implement task management service interface; improve error handling in global exception handler.
</commit_message>
<xml_diff>
--- a/data/chat-evaluation-QnA.xlsx
+++ b/data/chat-evaluation-QnA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hzy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hzy/projects/java/SpringHttpClientDataJpaDemo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D92932A-2998-CC4C-915D-8E78D2137CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D1AEB3-BD32-4446-96FC-1F801D992E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7DCE912F-E94F-1D47-AF47-D39C78B7FA2A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>question</t>
   </si>
@@ -55,16 +55,130 @@
   </si>
   <si>
     <t>golden_citations-1,golden_citations-2</t>
+  </si>
+  <si>
+    <t>question-2</t>
+  </si>
+  <si>
+    <t>golden_answer-2</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-3</t>
+  </si>
+  <si>
+    <t>question-3</t>
+  </si>
+  <si>
+    <t>golden_answer-3</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-4</t>
+  </si>
+  <si>
+    <t>question-4</t>
+  </si>
+  <si>
+    <t>golden_answer-4</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-5</t>
+  </si>
+  <si>
+    <t>question-5</t>
+  </si>
+  <si>
+    <t>golden_answer-5</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-6</t>
+  </si>
+  <si>
+    <t>question-6</t>
+  </si>
+  <si>
+    <t>golden_answer-6</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-7</t>
+  </si>
+  <si>
+    <t>question-7</t>
+  </si>
+  <si>
+    <t>golden_answer-7</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-8</t>
+  </si>
+  <si>
+    <t>question-8</t>
+  </si>
+  <si>
+    <t>golden_answer-8</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-9</t>
+  </si>
+  <si>
+    <t>question-9</t>
+  </si>
+  <si>
+    <t>golden_answer-9</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-10</t>
+  </si>
+  <si>
+    <t>question-10</t>
+  </si>
+  <si>
+    <t>golden_answer-10</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-11</t>
+  </si>
+  <si>
+    <t>question-11</t>
+  </si>
+  <si>
+    <t>golden_answer-11</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-12</t>
+  </si>
+  <si>
+    <t>question-12</t>
+  </si>
+  <si>
+    <t>golden_answer-12</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-13</t>
+  </si>
+  <si>
+    <t>question-0</t>
+  </si>
+  <si>
+    <t>golden_answer-0</t>
+  </si>
+  <si>
+    <t>golden_citations-1,golden_citations-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -427,10 +541,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A82BDE-112F-5E43-A9D4-A8B5F0EB138E}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,16 +562,149 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -465,10 +712,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ABDAA0-5254-4249-BBFC-5BEA94742691}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,16 +733,127 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement cursor-based pagination for task listing in TaskController and TaskApplicationService. Update TaskListResponse to include next_cursor and has_more fields for improved metadata. Modify TaskRepository to support cursor-based queries and adjust API documentation accordingly. Enhance error handling in GlobalExceptionHandler for validation and type mismatch exceptions.
</commit_message>
<xml_diff>
--- a/data/chat-evaluation-QnA.xlsx
+++ b/data/chat-evaluation-QnA.xlsx
@@ -8,13 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hzy/projects/java/SpringHttpClientDataJpaDemo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D1AEB3-BD32-4446-96FC-1F801D992E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99F537A-A47B-384C-9594-A2482284AA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{7DCE912F-E94F-1D47-AF47-D39C78B7FA2A}"/>
+    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" activeTab="8" xr2:uid="{7DCE912F-E94F-1D47-AF47-D39C78B7FA2A}"/>
   </bookViews>
   <sheets>
     <sheet name="uc-1" sheetId="1" r:id="rId1"/>
     <sheet name="uc-2" sheetId="2" r:id="rId2"/>
+    <sheet name="uc-2 (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="uc-2 (3)" sheetId="4" r:id="rId4"/>
+    <sheet name="uc-2 (4)" sheetId="5" r:id="rId5"/>
+    <sheet name="uc-2 (5)" sheetId="6" r:id="rId6"/>
+    <sheet name="uc-2 (6)" sheetId="7" r:id="rId7"/>
+    <sheet name="uc-2 (7)" sheetId="8" r:id="rId8"/>
+    <sheet name="uc-2 (8)" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="42">
   <si>
     <t>question</t>
   </si>
@@ -714,7 +721,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -856,4 +863,1033 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{089CB95C-FB4F-214C-AE85-788421E97A86}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8230A0D1-E4C2-E64A-BA3B-828DCEF47F84}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D94ABC-8D94-5D44-843F-8CF177925C73}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE211FE1-9D31-FE47-9DBB-0EF5A4C5045A}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7ECAD1-DB2E-564D-A93B-26BBE79A19C5}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42398ED1-8961-A049-95F5-3637020D9CF6}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7479D4-A439-7847-A10F-6501C98CBD9E}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>